<commit_message>
Editorial correction on the numbering of the CriteriaTaxonomy spread-sheets.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estaromi\OneDrive - everis\Projects\GROW\ESPD-EDM-v2.0.3\cl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\espd\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15376,9 +15376,7 @@
   <sheetPr codeName="Hoja12"/>
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -21500,9 +21498,7 @@
   <sheetPr codeName="Hoja19"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -22410,7 +22406,7 @@
   </sheetPr>
   <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -25902,7 +25898,7 @@
   <sheetPr codeName="Hoja20"/>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -28335,7 +28331,7 @@
   <sheetPr codeName="Hoja21"/>
   <dimension ref="A1:Z98"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -37152,9 +37148,7 @@
   <sheetPr codeName="Hoja25"/>
   <dimension ref="A1:AX26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -41157,7 +41151,7 @@
   <sheetPr codeName="Hoja27"/>
   <dimension ref="A1:AX141"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -56288,9 +56282,7 @@
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -57821,7 +57813,7 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:AX98"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -63167,7 +63159,7 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:AX44"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -66038,7 +66030,7 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:AX34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -68084,7 +68076,7 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -69337,7 +69329,7 @@
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -70090,7 +70082,7 @@
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:AX23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>